<commit_message>
language login sign up
</commit_message>
<xml_diff>
--- a/Mock chat Demo.xlsx
+++ b/Mock chat Demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Flutter\Rikkei\mock_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7B09A6-B31C-47AE-A007-7F9EA42A1F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A8BDEC-5ED1-4A2F-B27E-05BBD084AB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2580" windowWidth="13200" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13770" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Translation" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="105">
   <si>
     <t>key</t>
   </si>
@@ -28,27 +28,6 @@
     <t>en-US</t>
   </si>
   <si>
-    <t>vi_VN</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>Xin Chào</t>
-  </si>
-  <si>
-    <t>Welcome {}</t>
-  </si>
-  <si>
-    <t>ChaoMung {}</t>
-  </si>
-  <si>
-    <t>welcome-name</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -224,6 +203,138 @@
   </si>
   <si>
     <t>Search messages…</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Don't have an account?</t>
+  </si>
+  <si>
+    <t>Sign up now</t>
+  </si>
+  <si>
+    <t>Forgot your password?</t>
+  </si>
+  <si>
+    <t>Sign up</t>
+  </si>
+  <si>
+    <t>Already have an account?</t>
+  </si>
+  <si>
+    <t>Sign in now</t>
+  </si>
+  <si>
+    <t>terms</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>Chưa có tài khoản?</t>
+  </si>
+  <si>
+    <t>Đăng ký ngay</t>
+  </si>
+  <si>
+    <t>Quên mật khẩu?</t>
+  </si>
+  <si>
+    <t>Đăng ký</t>
+  </si>
+  <si>
+    <t>Đã có tài khoản?</t>
+  </si>
+  <si>
+    <t>Đăng nhập ngay</t>
+  </si>
+  <si>
+    <t>I agree to the</t>
+  </si>
+  <si>
+    <t>Tôi đồng ý với</t>
+  </si>
+  <si>
+    <t>policies</t>
+  </si>
+  <si>
+    <t>và</t>
+  </si>
+  <si>
+    <t>điều khoản</t>
+  </si>
+  <si>
+    <t>chính sách</t>
+  </si>
+  <si>
+    <t>SignUpNow</t>
+  </si>
+  <si>
+    <t>ForgotYourPassword</t>
+  </si>
+  <si>
+    <t>SignUp</t>
+  </si>
+  <si>
+    <t>IagreeToThe</t>
+  </si>
+  <si>
+    <t>vi-VN</t>
+  </si>
+  <si>
+    <t>Policies</t>
+  </si>
+  <si>
+    <t>And</t>
+  </si>
+  <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>AlreadyHaveAnAccount</t>
+  </si>
+  <si>
+    <t>SignInNow</t>
+  </si>
+  <si>
+    <t>DoNotHaveAnAccount</t>
+  </si>
+  <si>
+    <t>Trải nghiệm Awesome chat</t>
+  </si>
+  <si>
+    <t>Experience Awesome chat</t>
+  </si>
+  <si>
+    <t>Enter your email</t>
+  </si>
+  <si>
+    <t>Nhập email của bạn</t>
+  </si>
+  <si>
+    <t>EnterYourEmail</t>
+  </si>
+  <si>
+    <t>EnterYourPassword</t>
+  </si>
+  <si>
+    <t>Nhập mật khẩu của bạn</t>
+  </si>
+  <si>
+    <t>Enter your password</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Mật khẩu</t>
   </si>
 </sst>
 </file>
@@ -270,10 +381,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -492,20 +602,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
     <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,40 +623,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -554,244 +664,388 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
         <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
         <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>